<commit_message>
More changes to the excel sheet
</commit_message>
<xml_diff>
--- a/Documents/Proj1_control_signals.xlsx
+++ b/Documents/Proj1_control_signals.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colto\Desktop\CprE 381\CprE381\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colto\Desktop\CprE381\CprE381\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094B6A36-3A5D-4461-87F2-3F4054697E4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4F815F-0E98-4ADD-A7B6-D8421192D7BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00D6E995-B1C9-9941-8016-EE5CE3EB0628}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00D6E995-B1C9-9941-8016-EE5CE3EB0628}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="101">
   <si>
     <t>Instruction</t>
   </si>
@@ -242,18 +242,9 @@
     <t>1 is signed value, 0 is unsigned value</t>
   </si>
   <si>
-    <t>subi</t>
-  </si>
-  <si>
-    <t>subiu</t>
-  </si>
-  <si>
     <t>"0001"</t>
   </si>
   <si>
-    <t>"1111"</t>
-  </si>
-  <si>
     <t>"0000"</t>
   </si>
   <si>
@@ -330,6 +321,18 @@
   </si>
   <si>
     <t>1 is jumping, 0 means not</t>
+  </si>
+  <si>
+    <t>"001011"</t>
+  </si>
+  <si>
+    <t>Opcode</t>
+  </si>
+  <si>
+    <t>*These two don't have the 4th bit equal to 1 because of branching</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -382,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -400,14 +403,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -442,7 +448,7 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:rowOff>93345</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -779,13 +785,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FC2FCD1-6A91-3E43-87BE-182EA48A4800}">
-  <dimension ref="A1:R50"/>
+  <dimension ref="A1:R48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L6" sqref="L6"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -805,42 +811,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
     </row>
     <row r="2" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>62</v>
@@ -858,16 +864,16 @@
         <v>69</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
@@ -890,10 +896,10 @@
         <v>68</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>7</v>
@@ -913,7 +919,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -954,7 +960,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F5" s="3">
         <v>0</v>
@@ -968,8 +974,8 @@
       <c r="I5" s="3">
         <v>1</v>
       </c>
-      <c r="J5" s="5">
-        <v>1</v>
+      <c r="J5" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="K5" s="5">
         <v>0</v>
@@ -993,7 +999,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
@@ -1007,8 +1013,8 @@
       <c r="I6" s="1">
         <v>1</v>
       </c>
-      <c r="J6" s="5">
-        <v>0</v>
+      <c r="J6" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="K6" s="5">
         <v>0</v>
@@ -1031,7 +1037,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F7" s="1">
         <v>0</v>
@@ -1069,7 +1075,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F8" s="1">
         <v>0</v>
@@ -1083,8 +1089,8 @@
       <c r="I8" s="1">
         <v>1</v>
       </c>
-      <c r="J8" s="5">
-        <v>1</v>
+      <c r="J8" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="K8" s="5">
         <v>0</v>
@@ -1107,7 +1113,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F9" s="1">
         <v>0</v>
@@ -1145,7 +1151,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
@@ -1183,7 +1189,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
@@ -1221,7 +1227,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
@@ -1235,8 +1241,8 @@
       <c r="I12" s="1">
         <v>1</v>
       </c>
-      <c r="J12" s="5">
-        <v>0</v>
+      <c r="J12" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="K12" s="5">
         <v>0</v>
@@ -1259,7 +1265,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
@@ -1273,8 +1279,8 @@
       <c r="I13" s="1">
         <v>1</v>
       </c>
-      <c r="J13" s="5">
-        <v>0</v>
+      <c r="J13" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="K13" s="5">
         <v>0</v>
@@ -1297,7 +1303,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
@@ -1335,7 +1341,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F15" s="1">
         <v>0</v>
@@ -1349,8 +1355,8 @@
       <c r="I15" s="1">
         <v>1</v>
       </c>
-      <c r="J15" s="5">
-        <v>0</v>
+      <c r="J15" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="K15" s="5">
         <v>0</v>
@@ -1369,9 +1375,11 @@
       <c r="C16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D16"/>
+      <c r="D16" s="6">
+        <v>1</v>
+      </c>
       <c r="E16" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
@@ -1409,7 +1417,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>
@@ -1423,8 +1431,8 @@
       <c r="I17" s="1">
         <v>1</v>
       </c>
-      <c r="J17" s="5">
-        <v>0</v>
+      <c r="J17" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="K17" s="5">
         <v>0</v>
@@ -1447,7 +1455,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F18" s="1">
         <v>0</v>
@@ -1485,7 +1493,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F19" s="1">
         <v>0</v>
@@ -1499,8 +1507,8 @@
       <c r="I19" s="1">
         <v>1</v>
       </c>
-      <c r="J19" s="5">
-        <v>0</v>
+      <c r="J19" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="K19" s="5">
         <v>0</v>
@@ -1523,7 +1531,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F20" s="1">
         <v>0</v>
@@ -1537,8 +1545,8 @@
       <c r="I20" s="1">
         <v>1</v>
       </c>
-      <c r="J20" s="5">
-        <v>1</v>
+      <c r="J20" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="K20" s="5">
         <v>0</v>
@@ -1561,7 +1569,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
@@ -1575,8 +1583,8 @@
       <c r="I21" s="1">
         <v>1</v>
       </c>
-      <c r="J21" s="5">
-        <v>0</v>
+      <c r="J21" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="K21" s="5">
         <v>0</v>
@@ -1599,7 +1607,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F22" s="1">
         <v>1</v>
@@ -1637,7 +1645,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F23" s="1">
         <v>0</v>
@@ -1651,8 +1659,8 @@
       <c r="I23" s="1">
         <v>1</v>
       </c>
-      <c r="J23" s="5">
-        <v>1</v>
+      <c r="J23" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="K23" s="5">
         <v>0</v>
@@ -1675,7 +1683,7 @@
         <v>0</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F24" s="1">
         <v>0</v>
@@ -1689,8 +1697,8 @@
       <c r="I24" s="1">
         <v>1</v>
       </c>
-      <c r="J24" s="5">
-        <v>0</v>
+      <c r="J24" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="K24" s="5">
         <v>0</v>
@@ -1713,7 +1721,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F25" s="1">
         <v>0</v>
@@ -1751,7 +1759,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F26" s="1">
         <v>0</v>
@@ -1789,7 +1797,7 @@
         <v>0</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F27" s="1">
         <v>0</v>
@@ -1827,7 +1835,7 @@
         <v>0</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F28" s="1">
         <v>0</v>
@@ -1865,7 +1873,7 @@
         <v>0</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F29" s="1">
         <v>0</v>
@@ -1879,8 +1887,8 @@
       <c r="I29" s="1">
         <v>0</v>
       </c>
-      <c r="J29" s="5">
-        <v>0</v>
+      <c r="J29" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="K29" s="5">
         <v>1</v>
@@ -1903,7 +1911,7 @@
         <v>54</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>54</v>
@@ -1929,42 +1937,47 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" s="10" t="s">
+      <c r="A34" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
+        <v>71</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1972,116 +1985,139 @@
         <v>16</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>71</v>
+        <v>18</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>84</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E46" s="7"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>85</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E47" s="7"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>73</v>
+        <v>83</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>